<commit_message>
add hwacha textures, many updates to vehicleTypes cleaning things up. Also, rockets.
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="70">
   <si>
     <t>vehicle</t>
   </si>
@@ -206,13 +206,34 @@
   </si>
   <si>
     <t>blank</t>
+  </si>
+  <si>
+    <t>chest cart</t>
+  </si>
+  <si>
+    <t>% done</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>sz</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>ac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,14 +262,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -327,6 +356,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -361,6 +391,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -536,17 +567,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="6" width="3.28515625" customWidth="1"/>
     <col min="7" max="7" width="2.5703125" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
@@ -569,9 +600,10 @@
     <col min="29" max="29" width="2.7109375" customWidth="1"/>
     <col min="30" max="30" width="3.28515625" customWidth="1"/>
     <col min="31" max="31" width="2.5703125" customWidth="1"/>
+    <col min="32" max="32" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>34</v>
       </c>
@@ -638,8 +670,14 @@
       <c r="AB1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:31">
+      <c r="AF1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -733,8 +771,14 @@
       <c r="AE2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:31">
+      <c r="AF2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -777,6 +821,9 @@
       <c r="N3" t="s">
         <v>41</v>
       </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
       <c r="R3" t="s">
         <v>41</v>
       </c>
@@ -798,6 +845,9 @@
       <c r="X3" t="s">
         <v>41</v>
       </c>
+      <c r="Z3" t="s">
+        <v>41</v>
+      </c>
       <c r="AA3" t="s">
         <v>41</v>
       </c>
@@ -814,7 +864,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -854,6 +904,9 @@
       <c r="N4" t="s">
         <v>41</v>
       </c>
+      <c r="Q4" t="s">
+        <v>41</v>
+      </c>
       <c r="R4" t="s">
         <v>41</v>
       </c>
@@ -875,6 +928,9 @@
       <c r="X4" t="s">
         <v>41</v>
       </c>
+      <c r="Z4" t="s">
+        <v>41</v>
+      </c>
       <c r="AA4" t="s">
         <v>41</v>
       </c>
@@ -891,7 +947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -931,12 +987,21 @@
       <c r="N5" t="s">
         <v>41</v>
       </c>
+      <c r="Q5" t="s">
+        <v>41</v>
+      </c>
       <c r="R5" t="s">
         <v>41</v>
       </c>
       <c r="S5" t="s">
         <v>41</v>
       </c>
+      <c r="T5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5" t="s">
+        <v>41</v>
+      </c>
       <c r="V5" t="s">
         <v>41</v>
       </c>
@@ -946,6 +1011,9 @@
       <c r="X5" t="s">
         <v>41</v>
       </c>
+      <c r="Z5" t="s">
+        <v>41</v>
+      </c>
       <c r="AA5" t="s">
         <v>41</v>
       </c>
@@ -962,7 +1030,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1002,12 +1070,21 @@
       <c r="N6" t="s">
         <v>41</v>
       </c>
+      <c r="Q6" t="s">
+        <v>41</v>
+      </c>
       <c r="R6" t="s">
         <v>41</v>
       </c>
       <c r="S6" t="s">
         <v>41</v>
       </c>
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" t="s">
+        <v>41</v>
+      </c>
       <c r="V6" t="s">
         <v>41</v>
       </c>
@@ -1017,6 +1094,9 @@
       <c r="X6" t="s">
         <v>41</v>
       </c>
+      <c r="Z6" t="s">
+        <v>41</v>
+      </c>
       <c r="AA6" t="s">
         <v>41</v>
       </c>
@@ -1033,7 +1113,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1049,6 +1129,9 @@
       <c r="E7" t="s">
         <v>41</v>
       </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
       <c r="G7" t="s">
         <v>41</v>
       </c>
@@ -1073,6 +1156,9 @@
       <c r="N7" t="s">
         <v>41</v>
       </c>
+      <c r="Q7" t="s">
+        <v>41</v>
+      </c>
       <c r="R7" t="s">
         <v>41</v>
       </c>
@@ -1110,7 +1196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1123,6 +1209,9 @@
       <c r="E8" t="s">
         <v>41</v>
       </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
       <c r="G8" t="s">
         <v>41</v>
       </c>
@@ -1147,6 +1236,9 @@
       <c r="N8" t="s">
         <v>41</v>
       </c>
+      <c r="Q8" t="s">
+        <v>41</v>
+      </c>
       <c r="R8" t="s">
         <v>41</v>
       </c>
@@ -1184,7 +1276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1197,6 +1289,9 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
       <c r="G9" t="s">
         <v>41</v>
       </c>
@@ -1221,12 +1316,21 @@
       <c r="N9" t="s">
         <v>41</v>
       </c>
+      <c r="Q9" t="s">
+        <v>41</v>
+      </c>
       <c r="R9" t="s">
         <v>41</v>
       </c>
       <c r="S9" t="s">
         <v>41</v>
       </c>
+      <c r="T9" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" t="s">
+        <v>41</v>
+      </c>
       <c r="V9" t="s">
         <v>41</v>
       </c>
@@ -1252,7 +1356,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1265,6 +1369,9 @@
       <c r="E10" t="s">
         <v>41</v>
       </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
       <c r="G10" t="s">
         <v>41</v>
       </c>
@@ -1289,12 +1396,21 @@
       <c r="N10" t="s">
         <v>41</v>
       </c>
+      <c r="Q10" t="s">
+        <v>41</v>
+      </c>
       <c r="R10" t="s">
         <v>41</v>
       </c>
       <c r="S10" t="s">
         <v>41</v>
       </c>
+      <c r="T10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U10" t="s">
+        <v>41</v>
+      </c>
       <c r="V10" t="s">
         <v>41</v>
       </c>
@@ -1320,7 +1436,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1336,6 +1452,9 @@
       <c r="E11" t="s">
         <v>41</v>
       </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
       <c r="G11" t="s">
         <v>41</v>
       </c>
@@ -1360,12 +1479,21 @@
       <c r="N11" t="s">
         <v>41</v>
       </c>
+      <c r="Q11" t="s">
+        <v>41</v>
+      </c>
       <c r="R11" t="s">
         <v>41</v>
       </c>
       <c r="S11" t="s">
         <v>41</v>
       </c>
+      <c r="T11" t="s">
+        <v>41</v>
+      </c>
+      <c r="U11" t="s">
+        <v>41</v>
+      </c>
       <c r="V11" t="s">
         <v>41</v>
       </c>
@@ -1397,7 +1525,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1407,6 +1535,9 @@
       <c r="C12" t="s">
         <v>41</v>
       </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
       <c r="E12" t="s">
         <v>41</v>
       </c>
@@ -1434,9 +1565,21 @@
       <c r="N12" t="s">
         <v>41</v>
       </c>
+      <c r="Q12" t="s">
+        <v>41</v>
+      </c>
       <c r="R12" t="s">
         <v>41</v>
       </c>
+      <c r="S12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T12" t="s">
+        <v>41</v>
+      </c>
+      <c r="U12" t="s">
+        <v>41</v>
+      </c>
       <c r="V12" t="s">
         <v>41</v>
       </c>
@@ -1449,14 +1592,29 @@
       <c r="AA12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:31">
+      <c r="AB12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
       </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
       <c r="E13" t="s">
         <v>41</v>
       </c>
@@ -1484,12 +1642,21 @@
       <c r="N13" t="s">
         <v>41</v>
       </c>
+      <c r="Q13" t="s">
+        <v>41</v>
+      </c>
       <c r="R13" t="s">
         <v>41</v>
       </c>
       <c r="S13" t="s">
         <v>41</v>
       </c>
+      <c r="T13" t="s">
+        <v>41</v>
+      </c>
+      <c r="U13" t="s">
+        <v>41</v>
+      </c>
       <c r="V13" t="s">
         <v>41</v>
       </c>
@@ -1502,14 +1669,29 @@
       <c r="AA13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="AB13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
       </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
       <c r="E14" t="s">
         <v>41</v>
       </c>
@@ -1537,9 +1719,21 @@
       <c r="N14" t="s">
         <v>41</v>
       </c>
+      <c r="Q14" t="s">
+        <v>41</v>
+      </c>
       <c r="R14" t="s">
         <v>41</v>
       </c>
+      <c r="S14" t="s">
+        <v>41</v>
+      </c>
+      <c r="T14" t="s">
+        <v>41</v>
+      </c>
+      <c r="U14" t="s">
+        <v>41</v>
+      </c>
       <c r="V14" t="s">
         <v>41</v>
       </c>
@@ -1552,8 +1746,20 @@
       <c r="AA14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="AB14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1563,8 +1769,77 @@
       <c r="C15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>41</v>
+      </c>
+      <c r="S15" t="s">
+        <v>41</v>
+      </c>
+      <c r="T15" t="s">
+        <v>41</v>
+      </c>
+      <c r="U15" t="s">
+        <v>41</v>
+      </c>
+      <c r="V15" t="s">
+        <v>41</v>
+      </c>
+      <c r="W15" t="s">
+        <v>41</v>
+      </c>
+      <c r="X15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1572,17 +1847,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1590,25 +1865,63 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24">
-        <f>COUNTIF(C3:AE19,"")</f>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <f>COUNTIF(C3:AG20,"")</f>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25">
-        <f>COUNTIF(C3:AE19, "x")</f>
-        <v>250</v>
-      </c>
+        <f>COUNTIF(C3:AG20, "x")</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26">
+        <f>C25/(C25+C24)</f>
+        <v>0.58602150537634412</v>
+      </c>
+      <c r="C26" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add trebuchets, chest-cart.  clean up a render-order bug in guiContainerAdvanced.  clean up many params in vehicles...getting close.
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="70">
   <si>
     <t>vehicle</t>
   </si>
@@ -262,11 +262,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +572,7 @@
   <dimension ref="A1:AG26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="AE21" sqref="AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,20 +588,21 @@
     <col min="15" max="15" width="3" customWidth="1"/>
     <col min="16" max="16" width="3.140625" customWidth="1"/>
     <col min="17" max="17" width="2.42578125" customWidth="1"/>
-    <col min="18" max="18" width="3.5703125" customWidth="1"/>
-    <col min="19" max="20" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" customWidth="1"/>
+    <col min="19" max="19" width="3" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" customWidth="1"/>
     <col min="21" max="21" width="3.140625" customWidth="1"/>
     <col min="22" max="22" width="3.28515625" customWidth="1"/>
-    <col min="23" max="23" width="3.42578125" customWidth="1"/>
-    <col min="24" max="24" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="3" customWidth="1"/>
+    <col min="24" max="24" width="2.5703125" customWidth="1"/>
     <col min="25" max="25" width="2.28515625" customWidth="1"/>
     <col min="26" max="26" width="2.5703125" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" customWidth="1"/>
+    <col min="27" max="27" width="2.42578125" customWidth="1"/>
     <col min="28" max="28" width="3" customWidth="1"/>
     <col min="29" max="29" width="2.7109375" customWidth="1"/>
     <col min="30" max="30" width="3.28515625" customWidth="1"/>
     <col min="31" max="31" width="2.5703125" customWidth="1"/>
-    <col min="32" max="32" width="2.85546875" customWidth="1"/>
+    <col min="32" max="33" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -845,6 +847,9 @@
       <c r="X3" t="s">
         <v>41</v>
       </c>
+      <c r="Y3" t="s">
+        <v>41</v>
+      </c>
       <c r="Z3" t="s">
         <v>41</v>
       </c>
@@ -928,6 +933,9 @@
       <c r="X4" t="s">
         <v>41</v>
       </c>
+      <c r="Y4" t="s">
+        <v>41</v>
+      </c>
       <c r="Z4" t="s">
         <v>41</v>
       </c>
@@ -1011,6 +1019,9 @@
       <c r="X5" t="s">
         <v>41</v>
       </c>
+      <c r="Y5" t="s">
+        <v>41</v>
+      </c>
       <c r="Z5" t="s">
         <v>41</v>
       </c>
@@ -1094,6 +1105,9 @@
       <c r="X6" t="s">
         <v>41</v>
       </c>
+      <c r="Y6" t="s">
+        <v>41</v>
+      </c>
       <c r="Z6" t="s">
         <v>41</v>
       </c>
@@ -1180,6 +1194,12 @@
       <c r="X7" t="s">
         <v>41</v>
       </c>
+      <c r="Y7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>41</v>
+      </c>
       <c r="AA7" t="s">
         <v>41</v>
       </c>
@@ -1260,6 +1280,12 @@
       <c r="X8" t="s">
         <v>41</v>
       </c>
+      <c r="Y8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>41</v>
+      </c>
       <c r="AA8" t="s">
         <v>41</v>
       </c>
@@ -1340,6 +1366,12 @@
       <c r="X9" t="s">
         <v>41</v>
       </c>
+      <c r="Y9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>41</v>
+      </c>
       <c r="AA9" t="s">
         <v>41</v>
       </c>
@@ -1420,6 +1452,12 @@
       <c r="X10" t="s">
         <v>41</v>
       </c>
+      <c r="Y10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>41</v>
+      </c>
       <c r="AA10" t="s">
         <v>41</v>
       </c>
@@ -1541,6 +1579,9 @@
       <c r="E12" t="s">
         <v>41</v>
       </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" t="s">
         <v>41</v>
       </c>
@@ -1587,6 +1628,12 @@
         <v>41</v>
       </c>
       <c r="X12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" t="s">
         <v>41</v>
       </c>
       <c r="AA12" t="s">
@@ -1618,6 +1665,9 @@
       <c r="E13" t="s">
         <v>41</v>
       </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
       <c r="G13" t="s">
         <v>41</v>
       </c>
@@ -1664,6 +1714,12 @@
         <v>41</v>
       </c>
       <c r="X13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z13" t="s">
         <v>41</v>
       </c>
       <c r="AA13" t="s">
@@ -1695,6 +1751,9 @@
       <c r="E14" t="s">
         <v>41</v>
       </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
       <c r="G14" t="s">
         <v>41</v>
       </c>
@@ -1741,6 +1800,12 @@
         <v>41</v>
       </c>
       <c r="X14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z14" t="s">
         <v>41</v>
       </c>
       <c r="AA14" t="s">
@@ -1775,6 +1840,9 @@
       <c r="E15" t="s">
         <v>41</v>
       </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
       <c r="G15" t="s">
         <v>41</v>
       </c>
@@ -1800,6 +1868,9 @@
         <v>41</v>
       </c>
       <c r="Q15" t="s">
+        <v>41</v>
+      </c>
+      <c r="R15" t="s">
         <v>41</v>
       </c>
       <c r="S15" t="s">
@@ -1846,58 +1917,452 @@
       <c r="B16" t="s">
         <v>3</v>
       </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" t="s">
+        <v>41</v>
+      </c>
+      <c r="U16" t="s">
+        <v>41</v>
+      </c>
+      <c r="V16" t="s">
+        <v>41</v>
+      </c>
+      <c r="W16" t="s">
+        <v>41</v>
+      </c>
+      <c r="X16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" t="s">
+        <v>41</v>
+      </c>
+      <c r="S17" t="s">
+        <v>41</v>
+      </c>
+      <c r="T17" t="s">
+        <v>41</v>
+      </c>
+      <c r="U17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17" t="s">
+        <v>41</v>
+      </c>
+      <c r="W17" t="s">
+        <v>41</v>
+      </c>
+      <c r="X17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>41</v>
+      </c>
+      <c r="R18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S18" t="s">
+        <v>41</v>
+      </c>
+      <c r="T18" t="s">
+        <v>41</v>
+      </c>
+      <c r="U18" t="s">
+        <v>41</v>
+      </c>
+      <c r="V18" t="s">
+        <v>41</v>
+      </c>
+      <c r="W18" t="s">
+        <v>41</v>
+      </c>
+      <c r="X18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>41</v>
+      </c>
+      <c r="R19" t="s">
+        <v>41</v>
+      </c>
+      <c r="S19" t="s">
+        <v>41</v>
+      </c>
+      <c r="T19" t="s">
+        <v>41</v>
+      </c>
+      <c r="U19" t="s">
+        <v>41</v>
+      </c>
+      <c r="V19" t="s">
+        <v>41</v>
+      </c>
+      <c r="W19" t="s">
+        <v>41</v>
+      </c>
+      <c r="X19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>41</v>
+      </c>
+      <c r="R20" t="s">
+        <v>41</v>
+      </c>
+      <c r="S20" t="s">
+        <v>41</v>
+      </c>
+      <c r="T20" t="s">
+        <v>41</v>
+      </c>
+      <c r="U20" t="s">
+        <v>41</v>
+      </c>
+      <c r="V20" t="s">
+        <v>41</v>
+      </c>
+      <c r="W20" t="s">
+        <v>41</v>
+      </c>
+      <c r="X20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD20" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24">
         <f>COUNTIF(C3:AG20,"")</f>
-        <v>231</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25">
         <f>COUNTIF(C3:AG20, "x")</f>
-        <v>327</v>
+        <v>480</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
       <c r="B26">
         <f>C25/(C25+C24)</f>
-        <v>0.58602150537634412</v>
+        <v>0.86021505376344087</v>
       </c>
       <c r="C26" s="1"/>
     </row>

</xml_diff>

<commit_message>
update vehicle BB/size, add inventory drop code.
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="70">
   <si>
     <t>vehicle</t>
   </si>
@@ -572,7 +572,7 @@
   <dimension ref="A1:AG26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,6 +868,9 @@
       <c r="AE3" t="s">
         <v>41</v>
       </c>
+      <c r="AF3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -954,6 +957,9 @@
       <c r="AE4" t="s">
         <v>41</v>
       </c>
+      <c r="AF4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1040,6 +1046,9 @@
       <c r="AE5" t="s">
         <v>41</v>
       </c>
+      <c r="AF5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1126,6 +1135,9 @@
       <c r="AE6" t="s">
         <v>41</v>
       </c>
+      <c r="AF6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1215,6 +1227,9 @@
       <c r="AE7" t="s">
         <v>41</v>
       </c>
+      <c r="AF7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1301,6 +1316,9 @@
       <c r="AE8" t="s">
         <v>41</v>
       </c>
+      <c r="AF8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -1387,6 +1405,9 @@
       <c r="AE9" t="s">
         <v>41</v>
       </c>
+      <c r="AF9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1473,6 +1494,9 @@
       <c r="AE10" t="s">
         <v>41</v>
       </c>
+      <c r="AF10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1562,6 +1586,9 @@
       <c r="AE11" t="s">
         <v>41</v>
       </c>
+      <c r="AF11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1651,6 +1678,9 @@
       <c r="AE12" t="s">
         <v>41</v>
       </c>
+      <c r="AF12" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1737,6 +1767,9 @@
       <c r="AE13" t="s">
         <v>41</v>
       </c>
+      <c r="AF13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1823,6 +1856,9 @@
       <c r="AE14" t="s">
         <v>41</v>
       </c>
+      <c r="AF14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1891,6 +1927,9 @@
       <c r="X15" t="s">
         <v>41</v>
       </c>
+      <c r="Y15" t="s">
+        <v>41</v>
+      </c>
       <c r="Z15" t="s">
         <v>41</v>
       </c>
@@ -1907,6 +1946,9 @@
         <v>41</v>
       </c>
       <c r="AE15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1977,7 +2019,9 @@
       <c r="X16" t="s">
         <v>41</v>
       </c>
-      <c r="Y16" s="2"/>
+      <c r="Y16" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="Z16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1996,8 +2040,11 @@
       <c r="AE16" t="s">
         <v>41</v>
       </c>
+      <c r="AF16" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -2061,7 +2108,9 @@
       <c r="X17" t="s">
         <v>41</v>
       </c>
-      <c r="Y17" s="2"/>
+      <c r="Y17" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="Z17" s="2" t="s">
         <v>41</v>
       </c>
@@ -2080,8 +2129,11 @@
       <c r="AE17" t="s">
         <v>41</v>
       </c>
+      <c r="AF17" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2197,9 @@
       <c r="X18" t="s">
         <v>41</v>
       </c>
-      <c r="Y18" s="2"/>
+      <c r="Y18" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="Z18" s="2" t="s">
         <v>41</v>
       </c>
@@ -2164,8 +2218,11 @@
       <c r="AE18" t="s">
         <v>41</v>
       </c>
+      <c r="AF18" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2232,7 +2289,9 @@
       <c r="X19" t="s">
         <v>41</v>
       </c>
-      <c r="Y19" s="2"/>
+      <c r="Y19" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="Z19" s="2" t="s">
         <v>41</v>
       </c>
@@ -2251,8 +2310,11 @@
       <c r="AE19" t="s">
         <v>41</v>
       </c>
+      <c r="AF19" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2337,32 +2399,38 @@
       <c r="AD20" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="AE20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24">
         <f>COUNTIF(C3:AG20,"")</f>
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25">
         <f>COUNTIF(C3:AG20, "x")</f>
-        <v>480</v>
+        <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
       <c r="B26">
         <f>C25/(C25+C24)</f>
-        <v>0.86021505376344087</v>
+        <v>0.90322580645161288</v>
       </c>
       <c r="C26" s="1"/>
     </row>

</xml_diff>

<commit_message>
work on adding ammo types.
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="vehicles" sheetId="1" r:id="rId1"/>
+    <sheet name="ammos" sheetId="2" r:id="rId2"/>
+    <sheet name="upgrades" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="170">
   <si>
     <t>vehicle</t>
   </si>
@@ -224,16 +227,316 @@
   </si>
   <si>
     <t>ac</t>
+  </si>
+  <si>
+    <t>typeName</t>
+  </si>
+  <si>
+    <t>stoneShot 10</t>
+  </si>
+  <si>
+    <t>stoneShot 25</t>
+  </si>
+  <si>
+    <t>stoneShot 50</t>
+  </si>
+  <si>
+    <t>type made</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>ballista bolt</t>
+  </si>
+  <si>
+    <t>ballista bolt fire</t>
+  </si>
+  <si>
+    <t>ballista bolt explosive tipped</t>
+  </si>
+  <si>
+    <t>ballista bolt heavy iron</t>
+  </si>
+  <si>
+    <t>hwacha rocket</t>
+  </si>
+  <si>
+    <t>hwacha rocket fire</t>
+  </si>
+  <si>
+    <t>hwacha rocket airburst</t>
+  </si>
+  <si>
+    <t>ironShot 5</t>
+  </si>
+  <si>
+    <t>ironShot 10</t>
+  </si>
+  <si>
+    <t>ironShot 15</t>
+  </si>
+  <si>
+    <t>fireShot 10</t>
+  </si>
+  <si>
+    <t>fireShot 25</t>
+  </si>
+  <si>
+    <t>fireShot 50</t>
+  </si>
+  <si>
+    <t>explosiveShot 25</t>
+  </si>
+  <si>
+    <t>explosiveShot 10</t>
+  </si>
+  <si>
+    <t>explosiveShot 50</t>
+  </si>
+  <si>
+    <t>HEShot 10</t>
+  </si>
+  <si>
+    <t>HEShot 25</t>
+  </si>
+  <si>
+    <t>HEShot 50</t>
+  </si>
+  <si>
+    <t>napalmShot 10</t>
+  </si>
+  <si>
+    <t>napalmShot 25</t>
+  </si>
+  <si>
+    <t>napalmShot 50</t>
+  </si>
+  <si>
+    <t>typeNum</t>
+  </si>
+  <si>
+    <t>arrow</t>
+  </si>
+  <si>
+    <t>arrowFire</t>
+  </si>
+  <si>
+    <t>clusterShot 25</t>
+  </si>
+  <si>
+    <t>clusterShot 50</t>
+  </si>
+  <si>
+    <t>canisterShot 10</t>
+  </si>
+  <si>
+    <t>canisterShot 15</t>
+  </si>
+  <si>
+    <t>canisterShot 5 (impact)</t>
+  </si>
+  <si>
+    <t>grapeShot 5</t>
+  </si>
+  <si>
+    <t>grapeShot 10</t>
+  </si>
+  <si>
+    <t>grapeShot 15</t>
+  </si>
+  <si>
+    <t>clusterShot 10 (impact)</t>
+  </si>
+  <si>
+    <t>tx</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>entDmg</t>
+  </si>
+  <si>
+    <t>vehDmg</t>
+  </si>
+  <si>
+    <t>dmgType</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>explosive</t>
+  </si>
+  <si>
+    <t>hwacha rocket explosive tipped</t>
+  </si>
+  <si>
+    <t>pebbleShot 10 (shotgun)</t>
+  </si>
+  <si>
+    <t>pebbleShot 25 (shotgun)</t>
+  </si>
+  <si>
+    <t>pebbleShot 50 (shotgun)</t>
+  </si>
+  <si>
+    <t>special notes</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>tootip</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>(damage varies by distance from center of explosion)</t>
+  </si>
+  <si>
+    <t>(if hit, they'll be standing in freaking lava..lol..)</t>
+  </si>
+  <si>
+    <t>ballShot</t>
+  </si>
+  <si>
+    <t>shot by cluster/pebble/canister/grape shots in great numbers (10-50)</t>
+  </si>
+  <si>
+    <t>spawns 10 ballShot on impact</t>
+  </si>
+  <si>
+    <t>spawns 25 ballShot on impact</t>
+  </si>
+  <si>
+    <t>spawns 50 ballShot on impact</t>
+  </si>
+  <si>
+    <t>shot in large numbers by catapult and trebuchet (10-50)</t>
+  </si>
+  <si>
+    <t>basic stone-shot</t>
+  </si>
+  <si>
+    <t>basic stone-shot -- destroys a single block</t>
+  </si>
+  <si>
+    <t>basic stone-shot -- destroys several blocks</t>
+  </si>
+  <si>
+    <t>spawns 10 ballShot when shot</t>
+  </si>
+  <si>
+    <t>spawns 25 ballShot when shot</t>
+  </si>
+  <si>
+    <t>spawns 50 ballShot when shot</t>
+  </si>
+  <si>
+    <t>light a single block on fire</t>
+  </si>
+  <si>
+    <t>light a X area on fire</t>
+  </si>
+  <si>
+    <t>light a HUGE FREAKING AREA ON FIRE</t>
+  </si>
+  <si>
+    <t>cannon version of stone shot 10</t>
+  </si>
+  <si>
+    <t>cannon version of stone shot 25</t>
+  </si>
+  <si>
+    <t>cannon version of stone shot 50</t>
+  </si>
+  <si>
+    <t>spawns 4 ballShot on airbust (burst 7-10 blocks above ground)</t>
+  </si>
+  <si>
+    <t>shot</t>
+  </si>
+  <si>
+    <t>rocket</t>
+  </si>
+  <si>
+    <t>stone</t>
+  </si>
+  <si>
+    <t>expl</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>nap</t>
+  </si>
+  <si>
+    <t>clust</t>
+  </si>
+  <si>
+    <t>pebb</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>arF</t>
+  </si>
+  <si>
+    <t>bolt</t>
+  </si>
+  <si>
+    <t>boltF</t>
+  </si>
+  <si>
+    <t>boltE</t>
+  </si>
+  <si>
+    <t>penetrating -- will go through X many blocks (T2 Ballista)</t>
+  </si>
+  <si>
+    <t>rocketF</t>
+  </si>
+  <si>
+    <t>rocketE</t>
+  </si>
+  <si>
+    <t>rocketA</t>
+  </si>
+  <si>
+    <t>ball</t>
+  </si>
+  <si>
+    <t>grape</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,7 +660,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -392,7 +694,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -568,14 +869,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
@@ -605,7 +906,7 @@
     <col min="32" max="33" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="C1" t="s">
         <v>34</v>
       </c>
@@ -679,7 +980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +1081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -872,7 +1173,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -961,7 +1262,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1351,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1139,7 +1440,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1231,7 +1532,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +1621,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1409,7 +1710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1498,7 +1799,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1590,7 +1891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1983,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1771,7 +2072,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -1860,7 +2161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1952,7 +2253,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2044,7 +2345,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -2133,7 +2434,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -2222,7 +2523,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2314,7 +2615,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2406,7 +2707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -2415,7 +2716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -2424,7 +2725,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2438,9 +2739,9 @@
   <conditionalFormatting sqref="B26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2457,4 +2758,1481 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="66.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0.25</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.25</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>0.25</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>0.25</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>25</v>
+      </c>
+      <c r="I12">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>50</v>
+      </c>
+      <c r="I13">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>0.25</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15">
+        <v>25</v>
+      </c>
+      <c r="G15">
+        <v>0.5</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+      <c r="J16" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <v>0.25</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>115</v>
+      </c>
+      <c r="K17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>0.5</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>0.25</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>0.5</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>0.25</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>0.25</v>
+      </c>
+      <c r="H24">
+        <v>25</v>
+      </c>
+      <c r="I24">
+        <v>25</v>
+      </c>
+      <c r="J24" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <v>0.6</v>
+      </c>
+      <c r="H25">
+        <v>50</v>
+      </c>
+      <c r="I25">
+        <v>50</v>
+      </c>
+      <c r="J25" t="s">
+        <v>115</v>
+      </c>
+      <c r="K25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>0.25</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>115</v>
+      </c>
+      <c r="K26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>0.25</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>115</v>
+      </c>
+      <c r="K27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28">
+        <v>15</v>
+      </c>
+      <c r="G28">
+        <v>0.6</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>115</v>
+      </c>
+      <c r="K28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>0.25</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>115</v>
+      </c>
+      <c r="K29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>0.25</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>115</v>
+      </c>
+      <c r="K30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" t="s">
+        <v>167</v>
+      </c>
+      <c r="F31">
+        <v>15</v>
+      </c>
+      <c r="G31">
+        <v>0.6</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>115</v>
+      </c>
+      <c r="K31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0.2</v>
+      </c>
+      <c r="H32">
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>115</v>
+      </c>
+      <c r="K32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33">
+        <v>1.2</v>
+      </c>
+      <c r="G33">
+        <v>0.2</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>0.3</v>
+      </c>
+      <c r="H34">
+        <v>18</v>
+      </c>
+      <c r="I34">
+        <v>18</v>
+      </c>
+      <c r="J34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>0.3</v>
+      </c>
+      <c r="H35">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <v>20</v>
+      </c>
+      <c r="J35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>0.3</v>
+      </c>
+      <c r="H36">
+        <v>15</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>0.6</v>
+      </c>
+      <c r="H37">
+        <v>30</v>
+      </c>
+      <c r="I37">
+        <v>30</v>
+      </c>
+      <c r="J37" t="s">
+        <v>115</v>
+      </c>
+      <c r="K37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>0.2</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38">
+        <v>6</v>
+      </c>
+      <c r="J38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>0.2</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>8</v>
+      </c>
+      <c r="J39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <v>0.2</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>6</v>
+      </c>
+      <c r="J40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" t="s">
+        <v>165</v>
+      </c>
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>0.2</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>115</v>
+      </c>
+      <c r="K41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0.05</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
+        <v>115</v>
+      </c>
+      <c r="K42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="15" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more work on ammo types, missile count-weight stuff should be in play now, need to finish the ammo and vehicle weights though.
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="1"/>
@@ -12,12 +12,12 @@
     <sheet name="upgrades" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="172">
   <si>
     <t>vehicle</t>
   </si>
@@ -235,12 +235,6 @@
     <t>stoneShot 10</t>
   </si>
   <si>
-    <t>stoneShot 25</t>
-  </si>
-  <si>
-    <t>stoneShot 50</t>
-  </si>
-  <si>
     <t>type made</t>
   </si>
   <si>
@@ -286,33 +280,15 @@
     <t>fireShot 50</t>
   </si>
   <si>
-    <t>explosiveShot 25</t>
-  </si>
-  <si>
     <t>explosiveShot 10</t>
   </si>
   <si>
-    <t>explosiveShot 50</t>
-  </si>
-  <si>
     <t>HEShot 10</t>
   </si>
   <si>
-    <t>HEShot 25</t>
-  </si>
-  <si>
-    <t>HEShot 50</t>
-  </si>
-  <si>
     <t>napalmShot 10</t>
   </si>
   <si>
-    <t>napalmShot 25</t>
-  </si>
-  <si>
-    <t>napalmShot 50</t>
-  </si>
-  <si>
     <t>typeNum</t>
   </si>
   <si>
@@ -322,12 +298,6 @@
     <t>arrowFire</t>
   </si>
   <si>
-    <t>clusterShot 25</t>
-  </si>
-  <si>
-    <t>clusterShot 50</t>
-  </si>
-  <si>
     <t>canisterShot 10</t>
   </si>
   <si>
@@ -379,12 +349,6 @@
     <t>pebbleShot 10 (shotgun)</t>
   </si>
   <si>
-    <t>pebbleShot 25 (shotgun)</t>
-  </si>
-  <si>
-    <t>pebbleShot 50 (shotgun)</t>
-  </si>
-  <si>
     <t>special notes</t>
   </si>
   <si>
@@ -527,16 +491,58 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>wgt</t>
+  </si>
+  <si>
+    <t>mwgt</t>
+  </si>
+  <si>
+    <t>stoneShot 15</t>
+  </si>
+  <si>
+    <t>stoneShot 30</t>
+  </si>
+  <si>
+    <t>explosiveShot 15</t>
+  </si>
+  <si>
+    <t>explosiveShot 30</t>
+  </si>
+  <si>
+    <t>HEShot 15</t>
+  </si>
+  <si>
+    <t>HEShot 30</t>
+  </si>
+  <si>
+    <t>napalmShot 15</t>
+  </si>
+  <si>
+    <t>napalmShot 30</t>
+  </si>
+  <si>
+    <t>clusterShot 15</t>
+  </si>
+  <si>
+    <t>clusterShot 30</t>
+  </si>
+  <si>
+    <t>pebbleShot 15 (shotgun)</t>
+  </si>
+  <si>
+    <t>pebbleShot 30 (shotgun)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,12 +551,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -565,12 +577,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,6 +673,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -694,6 +708,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -869,14 +884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+      <selection activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
@@ -906,7 +921,7 @@
     <col min="32" max="33" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>34</v>
       </c>
@@ -980,7 +995,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1080,8 +1095,14 @@
       <c r="AG2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:33">
+      <c r="AH2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1172,8 +1193,11 @@
       <c r="AF3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:33">
+      <c r="AI3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1261,8 +1285,11 @@
       <c r="AF4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:33">
+      <c r="AI4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1350,8 +1377,11 @@
       <c r="AF5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:33">
+      <c r="AI5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1439,8 +1469,11 @@
       <c r="AF6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:33">
+      <c r="AI6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1531,8 +1564,11 @@
       <c r="AF7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:33">
+      <c r="AI7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1620,8 +1656,11 @@
       <c r="AF8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:33">
+      <c r="AI8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1709,8 +1748,11 @@
       <c r="AF9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:33">
+      <c r="AI9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1798,8 +1840,11 @@
       <c r="AF10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:33">
+      <c r="AI10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1890,8 +1935,11 @@
       <c r="AF11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:33">
+      <c r="AI11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1982,8 +2030,11 @@
       <c r="AF12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:33">
+      <c r="AI12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -2071,8 +2122,11 @@
       <c r="AF13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:33">
+      <c r="AI13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -2160,8 +2214,11 @@
       <c r="AF14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:33">
+      <c r="AI14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2252,8 +2309,11 @@
       <c r="AF15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:33">
+      <c r="AI15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2344,8 +2404,11 @@
       <c r="AF16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:32">
+      <c r="AI16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -2433,8 +2496,11 @@
       <c r="AF17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:32">
+      <c r="AI17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -2522,8 +2588,11 @@
       <c r="AF18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:32">
+      <c r="AI18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2614,8 +2683,11 @@
       <c r="AF19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:32">
+      <c r="AI19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2706,32 +2778,35 @@
       <c r="AF20" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:32">
+      <c r="AI20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24">
-        <f>COUNTIF(C3:AG20,"")</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32">
+        <f>COUNTIF(C3:AI20,"")</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25">
-        <f>COUNTIF(C3:AG20, "x")</f>
-        <v>504</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32">
+        <f>COUNTIF(C3:AI20, "x")</f>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
       <c r="B26">
         <f>C25/(C25+C24)</f>
-        <v>0.90322580645161288</v>
+        <v>0.87878787878787878</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -2739,9 +2814,9 @@
   <conditionalFormatting sqref="B26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2761,14 +2836,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -2783,42 +2859,42 @@
     <col min="11" max="11" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -2829,10 +2905,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -2847,15 +2923,15 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -2864,33 +2940,33 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F3">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0.5</v>
       </c>
       <c r="H3">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I3">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -2899,33 +2975,33 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -2934,10 +3010,10 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -2952,15 +3028,15 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -2969,33 +3045,33 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>0.5</v>
       </c>
       <c r="H6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -3004,42 +3080,42 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -3054,88 +3130,88 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F9">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>0.5</v>
       </c>
       <c r="H9">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -3150,88 +3226,88 @@
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>164</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="F12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>0.5</v>
       </c>
       <c r="H12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="F13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J13" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3240,94 +3316,94 @@
         <v>0.25</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J14" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" t="s">
         <v>116</v>
       </c>
-      <c r="K14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F15">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>0.5</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" t="s">
         <v>116</v>
       </c>
-      <c r="K15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F16">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I16">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" t="s">
         <v>116</v>
       </c>
-      <c r="K16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3342,27 +3418,27 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G18">
         <v>0.5</v>
@@ -3374,27 +3450,27 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E19" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3406,24 +3482,24 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3438,27 +3514,27 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F21">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G21">
         <v>0.5</v>
@@ -3470,27 +3546,27 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3502,24 +3578,24 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C23">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -3534,24 +3610,24 @@
         <v>10</v>
       </c>
       <c r="J23" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E24" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -3560,30 +3636,30 @@
         <v>0.25</v>
       </c>
       <c r="H24">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I24">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="F25">
         <v>15</v>
@@ -3592,30 +3668,30 @@
         <v>0.6</v>
       </c>
       <c r="H25">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I25">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C26">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="F26">
         <v>5</v>
@@ -3630,24 +3706,24 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K26" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C27">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E27" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="F27">
         <v>10</v>
@@ -3662,24 +3738,24 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C28">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E28" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="F28">
         <v>15</v>
@@ -3694,24 +3770,24 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C29">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E29" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F29">
         <v>5</v>
@@ -3726,24 +3802,24 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C30">
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F30">
         <v>10</v>
@@ -3758,24 +3834,24 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C31">
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -3790,56 +3866,56 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32">
+        <v>91</v>
+      </c>
+      <c r="C32" s="3">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>1</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>0.2</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>8</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="3">
         <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C33">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F33">
         <v>1.2</v>
@@ -3848,30 +3924,30 @@
         <v>0.2</v>
       </c>
       <c r="H33">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I33">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J33" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C34">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F34">
         <v>5</v>
@@ -3886,21 +3962,21 @@
         <v>18</v>
       </c>
       <c r="J34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E35" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="F35">
         <v>5</v>
@@ -3915,21 +3991,21 @@
         <v>20</v>
       </c>
       <c r="J35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F36">
         <v>8</v>
@@ -3944,21 +4020,21 @@
         <v>20</v>
       </c>
       <c r="J36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F37">
         <v>10</v>
@@ -3973,24 +4049,24 @@
         <v>30</v>
       </c>
       <c r="J37" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K37" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38">
+        <v>78</v>
+      </c>
+      <c r="C38" s="3">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E38" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="F38">
         <v>2</v>
@@ -4005,21 +4081,21 @@
         <v>6</v>
       </c>
       <c r="J38" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C39">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -4034,21 +4110,21 @@
         <v>8</v>
       </c>
       <c r="J39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C40">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F40">
         <v>4</v>
@@ -4063,21 +4139,21 @@
         <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41">
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F41">
         <v>5</v>
@@ -4092,42 +4168,42 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42">
+        <v>117</v>
+      </c>
+      <c r="C42" s="3">
         <v>40</v>
       </c>
-      <c r="D42" t="s">
-        <v>148</v>
+      <c r="D42" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>0.05</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="3">
         <v>5</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="3">
         <v>5</v>
       </c>
-      <c r="J42" t="s">
-        <v>115</v>
+      <c r="J42" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="K42" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -4136,33 +4212,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4171,63 +4247,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="15" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
re-arrange missiles. add test canister shot. rework weight alg (WIP). lots more other work on missileTypes
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="177">
   <si>
     <t>vehicle</t>
   </si>
@@ -533,6 +533,21 @@
   </si>
   <si>
     <t>pebbleShot 30 (shotgun)</t>
+  </si>
+  <si>
+    <t>missile wg</t>
+  </si>
+  <si>
+    <t>veh mx wh</t>
+  </si>
+  <si>
+    <t>arrowIron</t>
+  </si>
+  <si>
+    <t>arrowIronFire</t>
+  </si>
+  <si>
+    <t>fireShot 30</t>
   </si>
 </sst>
 </file>
@@ -2812,6 +2827,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2822,14 +2845,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2837,11 +2852,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2910,16 +2925,16 @@
       <c r="E2" t="s">
         <v>138</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>10</v>
       </c>
       <c r="G2">
         <v>0.25</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>10</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>10</v>
       </c>
       <c r="J2" t="s">
@@ -2945,16 +2960,16 @@
       <c r="E3" t="s">
         <v>138</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>15</v>
       </c>
       <c r="G3">
         <v>0.5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>15</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>15</v>
       </c>
       <c r="J3" t="s">
@@ -2980,16 +2995,16 @@
       <c r="E4" t="s">
         <v>138</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>30</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>30</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>30</v>
       </c>
       <c r="J4" t="s">
@@ -3000,43 +3015,16 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0.25</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>106</v>
-      </c>
-      <c r="K5" t="s">
-        <v>129</v>
-      </c>
+      <c r="F5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -3051,27 +3039,27 @@
         <v>106</v>
       </c>
       <c r="F6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
         <v>106</v>
       </c>
       <c r="K6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -3086,27 +3074,30 @@
         <v>106</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
         <v>106</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -3115,62 +3106,38 @@
         <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G8">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K8" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F9">
-        <v>15</v>
-      </c>
-      <c r="G9">
-        <v>0.5</v>
-      </c>
-      <c r="H9">
-        <v>15</v>
-      </c>
-      <c r="I9">
-        <v>15</v>
-      </c>
-      <c r="J9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K9" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -3182,16 +3149,16 @@
         <v>139</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="H10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>107</v>
@@ -3202,7 +3169,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -3211,19 +3178,19 @@
         <v>136</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G11">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
         <v>107</v>
@@ -3234,7 +3201,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -3243,19 +3210,19 @@
         <v>136</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
         <v>107</v>
@@ -3265,40 +3232,13 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>165</v>
-      </c>
       <c r="C13">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" t="s">
-        <v>140</v>
-      </c>
-      <c r="F13">
-        <v>30</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>30</v>
-      </c>
-      <c r="I13">
-        <v>30</v>
-      </c>
-      <c r="J13" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -3307,7 +3247,7 @@
         <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3322,15 +3262,15 @@
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C15">
         <v>13</v>
@@ -3339,7 +3279,7 @@
         <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F15">
         <v>15</v>
@@ -3354,15 +3294,15 @@
         <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C16">
         <v>14</v>
@@ -3371,7 +3311,7 @@
         <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F16">
         <v>30</v>
@@ -3386,47 +3326,20 @@
         <v>30</v>
       </c>
       <c r="J16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>99</v>
-      </c>
       <c r="C17">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" t="s">
-        <v>142</v>
-      </c>
-      <c r="F17">
-        <v>10</v>
-      </c>
-      <c r="G17">
-        <v>0.25</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>105</v>
-      </c>
-      <c r="K17" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="C18">
         <v>16</v>
@@ -3435,30 +3348,30 @@
         <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C19">
         <v>17</v>
@@ -3467,30 +3380,30 @@
         <v>136</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="C20">
         <v>18</v>
@@ -3499,62 +3412,35 @@
         <v>136</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G20">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K20" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>170</v>
-      </c>
       <c r="C21">
         <v>19</v>
       </c>
-      <c r="D21" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21">
-        <v>15</v>
-      </c>
-      <c r="G21">
-        <v>0.5</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>105</v>
-      </c>
-      <c r="K21" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>99</v>
       </c>
       <c r="C22">
         <v>20</v>
@@ -3563,13 +3449,13 @@
         <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -3581,12 +3467,12 @@
         <v>105</v>
       </c>
       <c r="K22" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="C23">
         <v>21</v>
@@ -3595,30 +3481,30 @@
         <v>136</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G23">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H23">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>105</v>
       </c>
       <c r="K23" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
       <c r="C24">
         <v>22</v>
@@ -3627,62 +3513,38 @@
         <v>136</v>
       </c>
       <c r="E24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G24">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
         <v>105</v>
       </c>
       <c r="K24" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>83</v>
+      <c r="A25">
+        <v>25</v>
       </c>
       <c r="C25">
         <v>23</v>
       </c>
-      <c r="D25" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25">
-        <v>15</v>
-      </c>
-      <c r="G25">
-        <v>0.6</v>
-      </c>
-      <c r="H25">
-        <v>30</v>
-      </c>
-      <c r="I25">
-        <v>30</v>
-      </c>
-      <c r="J25" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C26">
         <v>24</v>
@@ -3691,10 +3553,10 @@
         <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G26">
         <v>0.25</v>
@@ -3709,12 +3571,12 @@
         <v>105</v>
       </c>
       <c r="K26" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>170</v>
       </c>
       <c r="C27">
         <v>25</v>
@@ -3723,13 +3585,13 @@
         <v>136</v>
       </c>
       <c r="E27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F27">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G27">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -3741,12 +3603,12 @@
         <v>105</v>
       </c>
       <c r="K27" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="C28">
         <v>26</v>
@@ -3755,13 +3617,13 @@
         <v>136</v>
       </c>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F28">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G28">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -3773,44 +3635,20 @@
         <v>105</v>
       </c>
       <c r="K28" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>96</v>
+      <c r="A29">
+        <v>25</v>
       </c>
       <c r="C29">
         <v>27</v>
       </c>
-      <c r="D29" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" t="s">
-        <v>155</v>
-      </c>
-      <c r="F29">
-        <v>5</v>
-      </c>
-      <c r="G29">
-        <v>0.25</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>105</v>
-      </c>
-      <c r="K29" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C30">
         <v>28</v>
@@ -3819,30 +3657,30 @@
         <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G30">
         <v>0.25</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J30" t="s">
         <v>105</v>
       </c>
       <c r="K30" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C31">
         <v>29</v>
@@ -3851,358 +3689,646 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>0.25</v>
+      </c>
+      <c r="H31">
         <v>15</v>
       </c>
-      <c r="G31">
-        <v>0.6</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
       <c r="I31">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J31" t="s">
         <v>105</v>
       </c>
       <c r="K31" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="3">
+        <v>83</v>
+      </c>
+      <c r="C32">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="H32" s="3">
-        <v>8</v>
-      </c>
-      <c r="I32" s="3">
-        <v>8</v>
+        <v>144</v>
+      </c>
+      <c r="F32">
+        <v>15</v>
+      </c>
+      <c r="G32">
+        <v>0.6</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+      <c r="I32">
+        <v>30</v>
       </c>
       <c r="J32" t="s">
         <v>105</v>
       </c>
       <c r="K32" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>92</v>
+      <c r="A33">
+        <v>25</v>
       </c>
       <c r="C33">
         <v>31</v>
       </c>
-      <c r="D33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33">
-        <v>1.2</v>
-      </c>
-      <c r="G33">
-        <v>0.2</v>
-      </c>
-      <c r="H33">
-        <v>6</v>
-      </c>
-      <c r="I33">
-        <v>6</v>
-      </c>
-      <c r="J33" t="s">
-        <v>106</v>
-      </c>
-      <c r="K33" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C34">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F34">
         <v>5</v>
       </c>
       <c r="G34">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="H34">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J34" t="s">
         <v>105</v>
       </c>
+      <c r="K34" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C35">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G35">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="H35">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="K35" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C36">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="E36" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F36">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G36">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="H36">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="K36" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>77</v>
+      <c r="A37">
+        <v>25</v>
       </c>
       <c r="C37">
         <v>35</v>
       </c>
-      <c r="D37" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" t="s">
-        <v>147</v>
-      </c>
-      <c r="F37">
-        <v>10</v>
-      </c>
-      <c r="G37">
-        <v>0.6</v>
-      </c>
-      <c r="H37">
-        <v>30</v>
-      </c>
-      <c r="I37">
-        <v>30</v>
-      </c>
-      <c r="J37" t="s">
-        <v>105</v>
-      </c>
-      <c r="K37" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="3">
+        <v>96</v>
+      </c>
+      <c r="C38">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G38">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H38">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J38" t="s">
         <v>105</v>
       </c>
+      <c r="K38" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C39">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G39">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="K39" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C40">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E40" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G40">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="H40">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="K40" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>80</v>
+      <c r="A41">
+        <v>25</v>
       </c>
       <c r="C41">
         <v>39</v>
       </c>
-      <c r="D41" t="s">
-        <v>137</v>
-      </c>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41">
-        <v>5</v>
-      </c>
-      <c r="G41">
-        <v>0.2</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>105</v>
-      </c>
-      <c r="K41" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>8</v>
+      </c>
+      <c r="I42" s="3">
+        <v>8</v>
+      </c>
+      <c r="J42" t="s">
+        <v>105</v>
+      </c>
+      <c r="K42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43">
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43">
+        <v>1.2</v>
+      </c>
+      <c r="G43">
+        <v>0.2</v>
+      </c>
+      <c r="H43">
+        <v>6</v>
+      </c>
+      <c r="I43">
+        <v>6</v>
+      </c>
+      <c r="J43" t="s">
+        <v>106</v>
+      </c>
+      <c r="K43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+      <c r="F44">
+        <v>1.6</v>
+      </c>
+      <c r="H44">
+        <v>12</v>
+      </c>
+      <c r="I44">
+        <v>12</v>
+      </c>
+      <c r="J44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45">
+        <v>43</v>
+      </c>
+      <c r="F45">
+        <v>1.8</v>
+      </c>
+      <c r="H45">
+        <v>10</v>
+      </c>
+      <c r="I45">
+        <v>10</v>
+      </c>
+      <c r="J45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <v>0.3</v>
+      </c>
+      <c r="H46">
+        <v>18</v>
+      </c>
+      <c r="I46">
+        <v>18</v>
+      </c>
+      <c r="J46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="s">
+        <v>148</v>
+      </c>
+      <c r="F47">
+        <v>5</v>
+      </c>
+      <c r="G47">
+        <v>0.3</v>
+      </c>
+      <c r="H47">
+        <v>20</v>
+      </c>
+      <c r="I47">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48">
+        <v>46</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48">
+        <v>8</v>
+      </c>
+      <c r="G48">
+        <v>0.3</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48">
+        <v>20</v>
+      </c>
+      <c r="J48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49">
+        <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49">
+        <v>10</v>
+      </c>
+      <c r="G49">
+        <v>0.6</v>
+      </c>
+      <c r="H49">
+        <v>30</v>
+      </c>
+      <c r="I49">
+        <v>30</v>
+      </c>
+      <c r="J49" t="s">
+        <v>105</v>
+      </c>
+      <c r="K49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" t="s">
+        <v>137</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>0.2</v>
+      </c>
+      <c r="H50">
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <v>6</v>
+      </c>
+      <c r="J50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51">
+        <v>49</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" t="s">
+        <v>151</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>0.2</v>
+      </c>
+      <c r="H51">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <v>8</v>
+      </c>
+      <c r="J51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" t="s">
+        <v>152</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>0.2</v>
+      </c>
+      <c r="H52">
+        <v>6</v>
+      </c>
+      <c r="I52">
+        <v>6</v>
+      </c>
+      <c r="J52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53">
+        <v>51</v>
+      </c>
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <v>0.2</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>105</v>
+      </c>
+      <c r="K53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="3">
-        <v>40</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="C54">
+        <v>52</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E54" t="s">
         <v>154</v>
       </c>
-      <c r="F42">
+      <c r="F54">
         <v>1</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G54" s="3">
         <v>0.05</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H54" s="3">
         <v>5</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I54" s="3">
         <v>5</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K54" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4248,10 +4374,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4259,12 +4385,12 @@
     <col min="1" max="15" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>41</v>
       </c>
@@ -4274,8 +4400,14 @@
       <c r="E3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>172</v>
+      </c>
+      <c r="T3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -4291,8 +4423,14 @@
       <c r="F4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>50</v>
+      </c>
+      <c r="T4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>41</v>
       </c>
@@ -4303,9 +4441,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>41</v>
+      </c>
+      <c r="S6">
+        <f>R4+T4</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <f>T4/S6</f>
+        <v>0.375</v>
+      </c>
+      <c r="U7">
+        <f>T7*2</f>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many more ammo types working. almost time to start working on textures. shots also need sizes set...
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vehicles" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="upgrades" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="182">
   <si>
     <t>vehicle</t>
   </si>
@@ -277,9 +277,6 @@
     <t>fireShot 25</t>
   </si>
   <si>
-    <t>fireShot 50</t>
-  </si>
-  <si>
     <t>explosiveShot 10</t>
   </si>
   <si>
@@ -557,16 +554,25 @@
   </si>
   <si>
     <t>penetrating -- will go through X many blocks</t>
+  </si>
+  <si>
+    <t>fireShot 45</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>range</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +703,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -731,6 +738,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -906,14 +914,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
@@ -943,7 +951,7 @@
     <col min="32" max="33" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>34</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1118,13 +1126,13 @@
         <v>69</v>
       </c>
       <c r="AH2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI2" t="s">
         <v>157</v>
       </c>
-      <c r="AI2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35">
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1219,7 +1227,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1311,7 +1319,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1495,7 +1503,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1590,7 +1598,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +1690,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +1782,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1866,7 +1874,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1961,7 +1969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2056,7 +2064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -2148,7 +2156,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -2240,7 +2248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2335,7 +2343,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2430,7 +2438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -2522,7 +2530,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -2614,7 +2622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2709,7 +2717,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2804,7 +2812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -2813,7 +2821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -2822,7 +2830,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2844,9 +2852,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2858,15 +2866,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -2881,7 +2889,7 @@
     <col min="11" max="11" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -2889,53 +2897,53 @@
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
         <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
       </c>
       <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
         <v>101</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>102</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
       <c r="K1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" t="s">
-        <v>138</v>
+      <c r="D2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="F2" s="3">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0.25</v>
       </c>
       <c r="H2" s="3">
@@ -2944,33 +2952,33 @@
       <c r="I2" s="3">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3">
+      <c r="J2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>138</v>
+      <c r="D3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="F3" s="3">
         <v>15</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>0.5</v>
       </c>
       <c r="H3" s="3">
@@ -2979,33 +2987,33 @@
       <c r="I3" s="3">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4">
+      <c r="J3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" t="s">
-        <v>138</v>
+      <c r="D4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="F4" s="3">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" s="3">
@@ -3014,348 +3022,390 @@
       <c r="I4" s="3">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
-        <v>105</v>
-      </c>
-      <c r="K4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="C5">
+      <c r="J4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
         <v>3</v>
       </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="3">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="3">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>30</v>
+      </c>
+      <c r="I8" s="3">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="3">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H10" s="3">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F6">
+      <c r="K10" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="3">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>15</v>
+      </c>
+      <c r="I11" s="3">
+        <v>15</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="D12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="3">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>30</v>
+      </c>
+      <c r="I12" s="3">
+        <v>30</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="3">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3">
         <v>0.25</v>
       </c>
-      <c r="H6">
+      <c r="H14" s="3">
         <v>10</v>
       </c>
-      <c r="I6">
+      <c r="I14" s="3">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J14" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="K14" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="3">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>15</v>
+      </c>
+      <c r="I15" s="3">
+        <v>15</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F7">
+      <c r="K15" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="3">
+        <v>30</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>30</v>
+      </c>
+      <c r="I16" s="3">
+        <v>30</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="G7">
-        <v>0.5</v>
-      </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>15</v>
-      </c>
-      <c r="J7" t="s">
-        <v>106</v>
-      </c>
-      <c r="K7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>30</v>
-      </c>
-      <c r="I8">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>106</v>
-      </c>
-      <c r="K8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>0.25</v>
-      </c>
-      <c r="H10">
-        <v>10</v>
-      </c>
-      <c r="I10">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11">
-        <v>15</v>
-      </c>
-      <c r="G11">
-        <v>0.5</v>
-      </c>
-      <c r="H11">
-        <v>15</v>
-      </c>
-      <c r="I11">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F12">
-        <v>30</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>30</v>
-      </c>
-      <c r="I12">
-        <v>30</v>
-      </c>
-      <c r="J12" t="s">
-        <v>107</v>
-      </c>
-      <c r="K12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="C13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>88</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14">
-        <v>10</v>
-      </c>
-      <c r="G14">
-        <v>0.25</v>
-      </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="I14">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>107</v>
-      </c>
-      <c r="K14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <v>15</v>
-      </c>
-      <c r="I15">
-        <v>15</v>
-      </c>
-      <c r="J15" t="s">
-        <v>107</v>
-      </c>
-      <c r="K15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F16">
-        <v>30</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>30</v>
-      </c>
-      <c r="I16">
-        <v>30</v>
-      </c>
-      <c r="J16" t="s">
-        <v>107</v>
-      </c>
-      <c r="K16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="C17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>89</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3370,24 +3420,24 @@
         <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F19">
         <v>15</v>
@@ -3402,24 +3452,24 @@
         <v>15</v>
       </c>
       <c r="J19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20">
         <v>30</v>
@@ -3434,29 +3484,29 @@
         <v>30</v>
       </c>
       <c r="J20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -3471,24 +3521,24 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F23">
         <v>15</v>
@@ -3503,24 +3553,24 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C24">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F24">
         <v>30</v>
@@ -3535,13 +3585,13 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -3549,18 +3599,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F26">
         <v>10</v>
@@ -3575,24 +3625,24 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F27">
         <v>15</v>
@@ -3607,24 +3657,24 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C28">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F28">
         <v>30</v>
@@ -3639,13 +3689,13 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -3653,7 +3703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -3661,10 +3711,10 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F30">
         <v>5</v>
@@ -3679,13 +3729,13 @@
         <v>10</v>
       </c>
       <c r="J30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3693,10 +3743,10 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F31">
         <v>10</v>
@@ -3711,13 +3761,13 @@
         <v>15</v>
       </c>
       <c r="J31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -3725,10 +3775,10 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F32">
         <v>15</v>
@@ -3743,13 +3793,13 @@
         <v>30</v>
       </c>
       <c r="J32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
@@ -3757,18 +3807,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F34">
         <v>5</v>
@@ -3783,24 +3833,24 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F35">
         <v>10</v>
@@ -3815,24 +3865,24 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F36">
         <v>15</v>
@@ -3847,13 +3897,13 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>25</v>
       </c>
@@ -3861,18 +3911,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F38">
         <v>5</v>
@@ -3887,24 +3937,24 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F39">
         <v>10</v>
@@ -3919,24 +3969,24 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K39" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F40">
         <v>15</v>
@@ -3951,13 +4001,13 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K40" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>25</v>
       </c>
@@ -3965,15 +4015,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42">
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E42" t="s">
         <v>17</v>
@@ -3991,24 +4041,24 @@
         <v>8</v>
       </c>
       <c r="J42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43">
         <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F43">
         <v>1.2</v>
@@ -4023,15 +4073,15 @@
         <v>6</v>
       </c>
       <c r="J43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C44">
         <v>42</v>
@@ -4046,15 +4096,15 @@
         <v>12</v>
       </c>
       <c r="J44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K44" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C45">
         <v>43</v>
@@ -4069,10 +4119,10 @@
         <v>10</v>
       </c>
       <c r="J45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -4080,10 +4130,10 @@
         <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -4098,10 +4148,10 @@
         <v>18</v>
       </c>
       <c r="J46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -4109,10 +4159,10 @@
         <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F47">
         <v>2.2000000000000002</v>
@@ -4127,10 +4177,10 @@
         <v>16</v>
       </c>
       <c r="J47" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -4138,10 +4188,10 @@
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F48">
         <v>2.6</v>
@@ -4156,10 +4206,10 @@
         <v>15</v>
       </c>
       <c r="J48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -4167,10 +4217,10 @@
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F49">
         <v>3</v>
@@ -4185,13 +4235,13 @@
         <v>25</v>
       </c>
       <c r="J49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -4199,10 +4249,10 @@
         <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F50">
         <v>2</v>
@@ -4217,10 +4267,10 @@
         <v>6</v>
       </c>
       <c r="J50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -4228,10 +4278,10 @@
         <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F51">
         <v>3</v>
@@ -4246,21 +4296,21 @@
         <v>8</v>
       </c>
       <c r="J51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52">
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F52">
         <v>4</v>
@@ -4275,10 +4325,10 @@
         <v>6</v>
       </c>
       <c r="J52" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -4286,10 +4336,10 @@
         <v>51</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F53">
         <v>5</v>
@@ -4304,24 +4354,24 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K53" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54">
         <v>52</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -4336,24 +4386,24 @@
         <v>5</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K54" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C55">
         <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -4368,7 +4418,7 @@
         <v>8</v>
       </c>
       <c r="J55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4377,33 +4427,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>113</v>
-      </c>
-      <c r="F1" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4412,52 +4462,52 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:U7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:U15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="15" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:21">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>41</v>
       </c>
       <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
+        <v>170</v>
+      </c>
+      <c r="T3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" t="s">
         <v>155</v>
       </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" t="s">
-        <v>171</v>
-      </c>
-      <c r="T3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21">
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>156</v>
-      </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
@@ -4469,18 +4519,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:21">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>41</v>
       </c>
@@ -4489,7 +4539,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:21">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="T7">
         <f>T4/S6</f>
         <v>0.375</v>
@@ -4497,6 +4547,23 @@
       <c r="U7">
         <f>T7*2</f>
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>180</v>
+      </c>
+      <c r="R14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>-90</v>
+      </c>
+      <c r="R15">
+        <f>90-Q15</f>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
much more work on cleaning up ammo types and general vehicle features cleanup.
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vehicles" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="upgrades" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -568,11 +568,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,7 +703,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -738,7 +737,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -914,14 +912,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
@@ -951,7 +949,7 @@
     <col min="32" max="33" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35">
       <c r="C1" t="s">
         <v>34</v>
       </c>
@@ -1025,7 +1023,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1130,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1225,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1319,7 +1317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1411,7 +1409,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1501,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1598,7 +1596,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1690,7 +1688,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1782,7 +1780,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +1872,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1969,7 +1967,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2064,7 +2062,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -2156,7 +2154,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -2248,7 +2246,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2343,7 +2341,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2438,7 +2436,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -2530,7 +2528,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -2622,7 +2620,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2717,7 +2715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2812,7 +2810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -2821,7 +2819,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -2830,7 +2828,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2852,9 +2850,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2866,15 +2864,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:K17"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53:K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -2889,7 +2887,7 @@
     <col min="11" max="11" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -2924,7 +2922,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -2959,7 +2957,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>158</v>
       </c>
@@ -2994,7 +2992,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>159</v>
       </c>
@@ -3029,7 +3027,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -3044,7 +3042,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
@@ -3079,7 +3077,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>85</v>
       </c>
@@ -3114,7 +3112,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>174</v>
       </c>
@@ -3149,7 +3147,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -3166,7 +3164,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>86</v>
       </c>
@@ -3199,7 +3197,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
         <v>160</v>
       </c>
@@ -3232,7 +3230,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
         <v>161</v>
       </c>
@@ -3265,7 +3263,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3280,7 +3278,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>87</v>
       </c>
@@ -3313,7 +3311,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
         <v>162</v>
       </c>
@@ -3346,7 +3344,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
         <v>163</v>
       </c>
@@ -3379,7 +3377,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -3394,7 +3392,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -3426,7 +3424,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -3458,7 +3456,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -3490,542 +3488,606 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>45</v>
+      </c>
       <c r="C21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:11">
+      <c r="A22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C22">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
         <v>20</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>10</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>0.25</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="3">
         <v>0</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:11">
+      <c r="A23" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C23">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>15</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>0.5</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>0</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C24">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>30</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>1</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:11">
+      <c r="A25" s="3">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <v>23</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3">
+        <v>24</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="3">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
         <v>25</v>
       </c>
-      <c r="C25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26">
-        <v>24</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D27" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F26">
+      <c r="F27" s="3">
+        <v>15</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
+        <v>26</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="3">
+        <v>30</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="3">
+        <v>45</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
+        <v>27</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
+        <v>28</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="3">
+        <v>5</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="3">
         <v>10</v>
       </c>
-      <c r="G26">
+      <c r="I30" s="3">
+        <v>10</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3">
+        <v>29</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="3">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3">
         <v>0.25</v>
       </c>
-      <c r="H26">
+      <c r="H31" s="3">
+        <v>15</v>
+      </c>
+      <c r="I31" s="3">
+        <v>15</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
+        <v>30</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="3">
+        <v>15</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H32" s="3">
+        <v>30</v>
+      </c>
+      <c r="I32" s="3">
+        <v>30</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="3">
+        <v>25</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3">
+        <v>31</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3">
+        <v>32</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H34" s="3">
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="I34" s="3">
         <v>0</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J34" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K34" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3">
+        <v>33</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="3">
+        <v>10</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3">
+        <v>34</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" s="3">
+        <v>15</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="3">
+        <v>25</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3">
+        <v>35</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3">
+        <v>36</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="3">
+        <v>5</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>168</v>
-      </c>
-      <c r="C27">
+    <row r="39" spans="1:11">
+      <c r="A39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3">
+        <v>37</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" s="3">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3">
+        <v>38</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F40" s="3">
+        <v>15</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="3">
         <v>25</v>
       </c>
-      <c r="D27" t="s">
-        <v>135</v>
-      </c>
-      <c r="E27" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27">
-        <v>15</v>
-      </c>
-      <c r="G27">
-        <v>0.5</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
-        <v>104</v>
-      </c>
-      <c r="K27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28">
-        <v>26</v>
-      </c>
-      <c r="D28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E28" t="s">
-        <v>142</v>
-      </c>
-      <c r="F28">
-        <v>30</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>104</v>
-      </c>
-      <c r="K28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>25</v>
-      </c>
-      <c r="C29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30">
-        <v>28</v>
-      </c>
-      <c r="D30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" t="s">
-        <v>143</v>
-      </c>
-      <c r="F30">
-        <v>5</v>
-      </c>
-      <c r="G30">
-        <v>0.25</v>
-      </c>
-      <c r="H30">
-        <v>10</v>
-      </c>
-      <c r="I30">
-        <v>10</v>
-      </c>
-      <c r="J30" t="s">
-        <v>104</v>
-      </c>
-      <c r="K30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" t="s">
-        <v>143</v>
-      </c>
-      <c r="F31">
-        <v>10</v>
-      </c>
-      <c r="G31">
-        <v>0.25</v>
-      </c>
-      <c r="H31">
-        <v>15</v>
-      </c>
-      <c r="I31">
-        <v>15</v>
-      </c>
-      <c r="J31" t="s">
-        <v>104</v>
-      </c>
-      <c r="K31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32">
-        <v>30</v>
-      </c>
-      <c r="D32" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" t="s">
-        <v>143</v>
-      </c>
-      <c r="F32">
-        <v>15</v>
-      </c>
-      <c r="G32">
-        <v>0.6</v>
-      </c>
-      <c r="H32">
-        <v>30</v>
-      </c>
-      <c r="I32">
-        <v>30</v>
-      </c>
-      <c r="J32" t="s">
-        <v>104</v>
-      </c>
-      <c r="K32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>25</v>
-      </c>
-      <c r="C33">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34">
-        <v>32</v>
-      </c>
-      <c r="D34" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34">
-        <v>5</v>
-      </c>
-      <c r="G34">
-        <v>0.25</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>104</v>
-      </c>
-      <c r="K34" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35">
-        <v>33</v>
-      </c>
-      <c r="D35" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" t="s">
-        <v>144</v>
-      </c>
-      <c r="F35">
-        <v>10</v>
-      </c>
-      <c r="G35">
-        <v>0.25</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>104</v>
-      </c>
-      <c r="K35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36">
-        <v>34</v>
-      </c>
-      <c r="D36" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F36">
-        <v>15</v>
-      </c>
-      <c r="G36">
-        <v>0.6</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36" t="s">
-        <v>104</v>
-      </c>
-      <c r="K36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>25</v>
-      </c>
-      <c r="C37">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" t="s">
-        <v>153</v>
-      </c>
-      <c r="F38">
-        <v>5</v>
-      </c>
-      <c r="G38">
-        <v>0.25</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>104</v>
-      </c>
-      <c r="K38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39">
-        <v>37</v>
-      </c>
-      <c r="D39" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" t="s">
-        <v>153</v>
-      </c>
-      <c r="F39">
-        <v>10</v>
-      </c>
-      <c r="G39">
-        <v>0.25</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>104</v>
-      </c>
-      <c r="K39" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40">
-        <v>38</v>
-      </c>
-      <c r="D40" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" t="s">
-        <v>153</v>
-      </c>
-      <c r="F40">
-        <v>15</v>
-      </c>
-      <c r="G40">
-        <v>0.6</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>104</v>
-      </c>
-      <c r="K40" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>25</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C42">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3">
         <v>40</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="3">
@@ -4040,340 +4102,365 @@
       <c r="I42" s="3">
         <v>8</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:11">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C43">
-        <v>41</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3">
+        <v>41</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>1.2</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0.2</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="3">
         <v>6</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="3">
         <v>6</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:11">
+      <c r="A44" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C44">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3">
         <v>42</v>
       </c>
-      <c r="F44">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
         <v>1.6</v>
       </c>
-      <c r="H44">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3">
         <v>12</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="3">
         <v>12</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:11">
+      <c r="A45" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C45">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3">
         <v>43</v>
       </c>
-      <c r="F45">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3">
         <v>1.8</v>
       </c>
-      <c r="H45">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3">
         <v>10</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="3">
         <v>10</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C46">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3">
         <v>44</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>2</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>0.3</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="3">
         <v>18</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="3">
         <v>18</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C47">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3">
         <v>45</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>0.3</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="3">
         <v>16</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="3">
         <v>16</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C48">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3">
         <v>46</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>2.6</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="3">
         <v>0.3</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="3">
         <v>15</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="3">
         <v>15</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C49">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3">
         <v>47</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>3</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>0.6</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="3">
         <v>25</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="3">
         <v>25</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K49" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:11">
+      <c r="A50" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C50">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3">
         <v>48</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>2</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="3">
         <v>0.2</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="3">
         <v>6</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="3">
         <v>6</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C51">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3">
         <v>49</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>3</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="3">
         <v>0.2</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="3">
         <v>8</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="3">
         <v>8</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C52">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3">
         <v>50</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>4</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="3">
         <v>0.2</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="3">
         <v>6</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="3">
         <v>6</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C53">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3">
         <v>51</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>5</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="3">
         <v>0.2</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="3">
         <v>0</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="3">
         <v>0</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K53" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:11">
+      <c r="A54" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C54">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3">
         <v>52</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>1</v>
       </c>
       <c r="G54" s="3">
@@ -4388,38 +4475,40 @@
       <c r="J54" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K54" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:11">
+      <c r="A55" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C55">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3">
         <v>53</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>1</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="3">
         <v>0.05</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="3">
         <v>8</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="3">
         <v>8</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="K55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4427,16 +4516,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -4462,24 +4551,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="15" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21">
       <c r="D2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21">
       <c r="C3" t="s">
         <v>41</v>
       </c>
@@ -4496,7 +4585,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -4519,7 +4608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21">
       <c r="C5" t="s">
         <v>41</v>
       </c>
@@ -4530,7 +4619,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21">
       <c r="D6" t="s">
         <v>41</v>
       </c>
@@ -4539,7 +4628,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21">
       <c r="T7">
         <f>T4/S6</f>
         <v>0.375</v>
@@ -4549,7 +4638,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21">
       <c r="Q14" t="s">
         <v>180</v>
       </c>
@@ -4557,7 +4646,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21">
       <c r="Q15">
         <v>-90</v>
       </c>

</xml_diff>

<commit_message>
ammo stuff mostly done. tiny bit of work cleaning up npc targetHelpers
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/vehicles todo table.xlsx
+++ b/AncientWarfare/project_resources/vehicles todo table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="16155" windowHeight="8445" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vehicles" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="upgrades" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="182">
   <si>
     <t>vehicle</t>
   </si>
@@ -568,11 +568,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,6 +703,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -737,6 +738,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -912,14 +914,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
@@ -949,7 +951,7 @@
     <col min="32" max="33" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>34</v>
       </c>
@@ -1023,7 +1025,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1225,7 +1227,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1501,7 +1503,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1596,7 +1598,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1688,7 +1690,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1872,7 +1874,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1967,7 +1969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2062,7 +2064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -2154,7 +2156,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -2246,7 +2248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2436,7 +2438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -2528,7 +2530,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -2620,7 +2622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2715,7 +2717,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2810,7 +2812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -2819,7 +2821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -2828,7 +2830,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2850,9 +2852,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2864,15 +2866,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A53" sqref="A53:K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -2887,7 +2889,7 @@
     <col min="11" max="11" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -2922,7 +2924,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -2957,7 +2959,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>158</v>
       </c>
@@ -2992,7 +2994,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>159</v>
       </c>
@@ -3027,7 +3029,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -3042,7 +3044,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
@@ -3077,7 +3079,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>85</v>
       </c>
@@ -3112,7 +3114,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>174</v>
       </c>
@@ -3147,7 +3149,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -3164,7 +3166,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>86</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>160</v>
       </c>
@@ -3230,7 +3232,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>161</v>
       </c>
@@ -3263,7 +3265,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -3278,7 +3280,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>87</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>162</v>
       </c>
@@ -3344,7 +3346,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>163</v>
       </c>
@@ -3377,7 +3379,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -3392,7 +3394,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -3424,7 +3426,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -3456,7 +3458,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -3488,7 +3490,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>45</v>
       </c>
@@ -3496,7 +3498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>98</v>
       </c>
@@ -3529,7 +3531,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>166</v>
       </c>
@@ -3562,7 +3564,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>167</v>
       </c>
@@ -3595,7 +3597,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>45</v>
       </c>
@@ -3612,7 +3614,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>108</v>
       </c>
@@ -3645,7 +3647,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>168</v>
       </c>
@@ -3678,7 +3680,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>169</v>
       </c>
@@ -3711,7 +3713,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>45</v>
       </c>
@@ -3728,7 +3730,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
@@ -3794,7 +3796,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
@@ -3827,7 +3829,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>25</v>
       </c>
@@ -3844,7 +3846,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
@@ -3877,7 +3879,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>92</v>
       </c>
@@ -3910,7 +3912,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>93</v>
       </c>
@@ -3943,7 +3945,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>25</v>
       </c>
@@ -3960,7 +3962,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>95</v>
       </c>
@@ -3993,7 +3995,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>96</v>
       </c>
@@ -4026,7 +4028,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>97</v>
       </c>
@@ -4059,7 +4061,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>25</v>
       </c>
@@ -4076,7 +4078,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>90</v>
       </c>
@@ -4109,7 +4111,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
@@ -4142,7 +4144,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>172</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>173</v>
       </c>
@@ -4194,7 +4196,7 @@
       </c>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>74</v>
       </c>
@@ -4225,7 +4227,7 @@
       </c>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>75</v>
       </c>
@@ -4256,7 +4258,7 @@
       </c>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>76</v>
       </c>
@@ -4287,7 +4289,7 @@
       </c>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>77</v>
       </c>
@@ -4320,7 +4322,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>78</v>
       </c>
@@ -4351,7 +4353,7 @@
       </c>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>79</v>
       </c>
@@ -4382,7 +4384,7 @@
       </c>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
@@ -4413,7 +4415,7 @@
       </c>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>80</v>
       </c>
@@ -4446,7 +4448,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>116</v>
       </c>
@@ -4479,7 +4481,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>176</v>
       </c>
@@ -4516,16 +4518,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -4551,24 +4553,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:U15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:X28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="15" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:21">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>41</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:21">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -4608,7 +4610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>41</v>
       </c>
@@ -4619,7 +4621,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:21">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>41</v>
       </c>
@@ -4628,7 +4630,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:21">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="T7">
         <f>T4/S6</f>
         <v>0.375</v>
@@ -4638,7 +4640,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="2:21">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="Q14" t="s">
         <v>180</v>
       </c>
@@ -4646,13 +4648,238 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="2:21">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="Q15">
         <v>-90</v>
       </c>
       <c r="R15">
         <f>90-Q15</f>
         <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <v>10</v>
+      </c>
+      <c r="U18">
+        <v>45</v>
+      </c>
+      <c r="V18">
+        <f>T18+U18</f>
+        <v>55</v>
+      </c>
+      <c r="W18">
+        <f>(T18/V18)*2</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="X18">
+        <f>T18/U18</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="19" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <v>15</v>
+      </c>
+      <c r="U19">
+        <v>45</v>
+      </c>
+      <c r="V19">
+        <f t="shared" ref="V19:V22" si="0">T19+U19</f>
+        <v>60</v>
+      </c>
+      <c r="W19">
+        <f t="shared" ref="W19:W22" si="1">(T19/V19)*2</f>
+        <v>0.5</v>
+      </c>
+      <c r="X19">
+        <f t="shared" ref="X19:X22" si="2">T19/U19</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="20" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <v>30</v>
+      </c>
+      <c r="U20">
+        <v>45</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>45</v>
+      </c>
+      <c r="U21">
+        <v>45</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>55</v>
+      </c>
+      <c r="U22">
+        <v>45</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="2"/>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="23" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <v>75</v>
+      </c>
+      <c r="U23">
+        <v>45</v>
+      </c>
+      <c r="V23">
+        <f t="shared" ref="V23:V28" si="3">T23+U23</f>
+        <v>120</v>
+      </c>
+      <c r="W23">
+        <f t="shared" ref="W23:W28" si="4">(T23/V23)*2</f>
+        <v>1.25</v>
+      </c>
+      <c r="X23">
+        <f t="shared" ref="X23:X28" si="5">T23/U23</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <v>90</v>
+      </c>
+      <c r="U24">
+        <v>45</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="4"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <v>125</v>
+      </c>
+      <c r="U25">
+        <v>45</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="4"/>
+        <v>1.4705882352941178</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="5"/>
+        <v>2.7777777777777777</v>
+      </c>
+    </row>
+    <row r="26" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <v>300</v>
+      </c>
+      <c r="U26">
+        <v>45</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="3"/>
+        <v>345</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="4"/>
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="5"/>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <v>450</v>
+      </c>
+      <c r="U27">
+        <v>45</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="3"/>
+        <v>495</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="4"/>
+        <v>1.8181818181818181</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="20:24" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <v>55</v>
+      </c>
+      <c r="U28">
+        <v>45</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="4"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="5"/>
+        <v>1.2222222222222223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>